<commit_message>
start doing changes for the revenue and expense as invoice comes in
</commit_message>
<xml_diff>
--- a/excel_templates/revenue-template.xlsx
+++ b/excel_templates/revenue-template.xlsx
@@ -19,21 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Revenue type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Amount</t>
-  </si>
-  <si>
-    <t>Start period</t>
-  </si>
-  <si>
-    <t>End period</t>
-  </si>
-  <si>
-    <t>Apartment</t>
   </si>
   <si>
     <t>Payment date</t>
@@ -44,6 +32,9 @@
   <si>
     <t>Note</t>
   </si>
+  <si>
+    <t>Invoice</t>
+  </si>
 </sst>
 </file>
 
@@ -52,7 +43,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -126,7 +117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -410,212 +401,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.7109375" customWidth="1"/>
+    <col min="1" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
innitialize the invoice fix, will continue fixing it.
</commit_message>
<xml_diff>
--- a/excel_templates/revenue-template.xlsx
+++ b/excel_templates/revenue-template.xlsx
@@ -33,7 +33,7 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Invoice</t>
+    <t>Lease Agreement</t>
   </si>
 </sst>
 </file>
@@ -404,15 +404,17 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>